<commit_message>
added auto-fill of combo boxes
</commit_message>
<xml_diff>
--- a/Connection_Configs/Connection_Configs.xlsx
+++ b/Connection_Configs/Connection_Configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79137\Pasha\Bachelor Thesis Project\Project\Connection_Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BE2D97-1115-4FB7-8016-9BCB28642100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DC343A-E359-40A0-9B0A-43C3D8D9F2F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21564" yWindow="2028" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Protocol</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>COM Port</t>
+  </si>
+  <si>
+    <t>COM3</t>
   </si>
 </sst>
 </file>
@@ -379,7 +382,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,8 +420,8 @@
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2">
-        <v>3</v>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
       <c r="F2">
         <v>9600</v>

</xml_diff>